<commit_message>
Final Parts List Spreadsheet
</commit_message>
<xml_diff>
--- a/Component_Docs/Station_Parts_List.xlsx
+++ b/Component_Docs/Station_Parts_List.xlsx
@@ -814,12 +814,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,7 +846,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="3" t="n">
-        <f aca="false">SUM(I3:I68)</f>
+        <f aca="false">SUM(I3:I31)</f>
         <v>463.11</v>
       </c>
       <c r="J1" s="1"/>
@@ -1853,297 +1853,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="n">
-        <f aca="false">+H32*G32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="4"/>
-      <c r="I33" s="4" t="n">
-        <f aca="false">+H33*G33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="4"/>
-      <c r="I34" s="4" t="n">
-        <f aca="false">+H34*G34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="n">
-        <f aca="false">+H35*G35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="4"/>
-      <c r="I36" s="4" t="n">
-        <f aca="false">+H36*G36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="4"/>
-      <c r="I37" s="4" t="n">
-        <f aca="false">+H37*G37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="n">
-        <f aca="false">+H38*G38</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="4"/>
-      <c r="I39" s="4" t="n">
-        <f aca="false">+H39*G39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="4"/>
-      <c r="I40" s="4" t="n">
-        <f aca="false">+H40*G40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="4"/>
-      <c r="I41" s="4" t="n">
-        <f aca="false">+H41*G41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="4"/>
-      <c r="I42" s="4" t="n">
-        <f aca="false">+H42*G42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="4"/>
-      <c r="I43" s="4" t="n">
-        <f aca="false">+H43*G43</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="4"/>
-      <c r="I44" s="4" t="n">
-        <f aca="false">+H44*G44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="4"/>
-      <c r="I45" s="4" t="n">
-        <f aca="false">+H45*G45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="4"/>
-      <c r="I46" s="4" t="n">
-        <f aca="false">+H46*G46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="4"/>
-      <c r="I47" s="4" t="n">
-        <f aca="false">+H47*G47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="4"/>
-      <c r="I48" s="4" t="n">
-        <f aca="false">+H48*G48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H49" s="4"/>
-      <c r="I49" s="4" t="n">
-        <f aca="false">+H49*G49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H50" s="4"/>
-      <c r="I50" s="4" t="n">
-        <f aca="false">+H50*G50</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H51" s="4"/>
-      <c r="I51" s="4" t="n">
-        <f aca="false">+H51*G51</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H52" s="4"/>
-      <c r="I52" s="4" t="n">
-        <f aca="false">+H52*G52</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H53" s="4"/>
-      <c r="I53" s="4" t="n">
-        <f aca="false">+H53*G53</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H54" s="4"/>
-      <c r="I54" s="4" t="n">
-        <f aca="false">+H54*G54</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H55" s="4"/>
-      <c r="I55" s="4" t="n">
-        <f aca="false">+H55*G55</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H56" s="4"/>
-      <c r="I56" s="4" t="n">
-        <f aca="false">+H56*G56</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="4"/>
-      <c r="I57" s="4" t="n">
-        <f aca="false">+H57*G57</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H58" s="4"/>
-      <c r="I58" s="4" t="n">
-        <f aca="false">+H58*G58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="4"/>
-      <c r="I59" s="4" t="n">
-        <f aca="false">+H59*G59</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="4"/>
-      <c r="I60" s="4" t="n">
-        <f aca="false">+H60*G60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H61" s="4"/>
-      <c r="I61" s="4" t="n">
-        <f aca="false">+H61*G61</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H62" s="4"/>
-      <c r="I62" s="4" t="n">
-        <f aca="false">+H62*G62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H63" s="4"/>
-      <c r="I63" s="4" t="n">
-        <f aca="false">+H63*G63</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H64" s="4"/>
-      <c r="I64" s="4" t="n">
-        <f aca="false">+H64*G64</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H65" s="4"/>
-      <c r="I65" s="4" t="n">
-        <f aca="false">+H65*G65</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H66" s="4"/>
-      <c r="I66" s="4" t="n">
-        <f aca="false">+H66*G66</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H67" s="4"/>
-      <c r="I67" s="4" t="n">
-        <f aca="false">+H67*G67</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H68" s="4"/>
-      <c r="I68" s="4" t="n">
-        <f aca="false">+H68*G68</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+    <row r="32" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="6" t="s">
+    <row r="33" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="6" t="s">
+    <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="6" t="s">
+    <row r="35" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="6" t="s">
+    <row r="36" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="6" t="s">
         <v>159</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>